<commit_message>
utlmos cambios de reporte de excel
</commit_message>
<xml_diff>
--- a/simple.xlsx
+++ b/simple.xlsx
@@ -67,27 +67,67 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.489887640449439"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.78988764044944"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="5.289887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>Cover</t>
+          <t>p1</t>
         </is>
       </c>
       <c r="B1" s="0" t="inlineStr">
         <is>
-          <t>Sheet</t>
+          <t>p2</t>
         </is>
       </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>p3</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>p4</t>
+        </is>
+      </c>
+      <c r="E1" s="0" t="inlineStr">
+        <is>
+          <t>p5</t>
+        </is>
+      </c>
+      <c r="F1" s="0" t="inlineStr">
+        <is>
+          <t>p6</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>algunas veces</t>
+        </is>
+      </c>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>

</xml_diff>